<commit_message>
added map of port liner connectivity index
</commit_message>
<xml_diff>
--- a/port_manual_berth.xlsx
+++ b/port_manual_berth.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="8040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="port_manual_berth" sheetId="1" r:id="rId1"/>
     <sheet name="google_earth_history" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">port_manual_berth!$A$1:$E$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">port_manual_berth!$A$1:$E$115</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="244">
   <si>
     <t>port</t>
   </si>
@@ -1569,10 +1569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:XFD98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1861,10 +1861,10 @@
         <v>106</v>
       </c>
       <c r="C17" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -1872,47 +1872,47 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="C18" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2">
         <v>7</v>
       </c>
       <c r="E18" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>154</v>
+        <v>70</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="C19" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2">
         <v>7</v>
       </c>
       <c r="E19" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>204</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>71</v>
+        <v>205</v>
       </c>
       <c r="C20" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2">
         <v>7</v>
@@ -1923,10 +1923,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C21" s="2">
         <v>6</v>
@@ -1940,13 +1940,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>195</v>
+        <v>72</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>196</v>
+        <v>73</v>
       </c>
       <c r="C22" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2">
         <v>7</v>
@@ -1957,13 +1957,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>189</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>190</v>
       </c>
       <c r="C23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" s="2">
         <v>7</v>
@@ -1974,16 +1974,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C24" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="2">
         <v>0</v>
@@ -1991,13 +1991,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>185</v>
+        <v>111</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>186</v>
+        <v>112</v>
       </c>
       <c r="C25" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D25" s="2">
         <v>6</v>
@@ -2008,13 +2008,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>111</v>
+        <v>191</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>112</v>
+        <v>192</v>
       </c>
       <c r="C26" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2">
         <v>6</v>
@@ -2025,13 +2025,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>191</v>
+        <v>115</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>192</v>
+        <v>116</v>
       </c>
       <c r="C27" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" s="2">
         <v>6</v>
@@ -2042,10 +2042,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="C28" s="2">
         <v>3</v>
@@ -2059,13 +2059,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C29" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" s="2">
         <v>6</v>
@@ -2076,13 +2076,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="C30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" s="2">
         <v>6</v>
@@ -2093,16 +2093,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="C31" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
@@ -2110,13 +2110,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>144</v>
+        <v>210</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>145</v>
+        <v>211</v>
       </c>
       <c r="C32" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2">
         <v>5</v>
@@ -2127,13 +2127,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>210</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>211</v>
+        <v>57</v>
       </c>
       <c r="C33" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2">
         <v>5</v>
@@ -2144,13 +2144,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C34" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34" s="2">
         <v>5</v>
@@ -2161,13 +2161,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
       <c r="C35" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" s="2">
         <v>5</v>
@@ -2178,13 +2178,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="C36" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="2">
         <v>5</v>
@@ -2195,13 +2195,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>179</v>
+        <v>86</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>180</v>
+        <v>87</v>
       </c>
       <c r="C37" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="2">
         <v>5</v>
@@ -2212,13 +2212,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="C38" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D38" s="2">
         <v>5</v>
@@ -2229,13 +2229,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>50</v>
+        <v>197</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>51</v>
+        <v>198</v>
       </c>
       <c r="C39" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39" s="2">
         <v>5</v>
@@ -2246,47 +2246,47 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="C40" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E40" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>231</v>
+        <v>68</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>232</v>
+        <v>69</v>
       </c>
       <c r="C41" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" s="2">
         <v>4</v>
       </c>
       <c r="E41" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>68</v>
+        <v>146</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
       <c r="C42" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D42" s="2">
         <v>4</v>
@@ -2297,13 +2297,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>146</v>
+        <v>208</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>147</v>
+        <v>209</v>
       </c>
       <c r="C43" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43" s="2">
         <v>4</v>
@@ -2314,13 +2314,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="C44" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44" s="2">
         <v>4</v>
@@ -2331,10 +2331,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>183</v>
+        <v>225</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="C45" s="2">
         <v>2</v>
@@ -2348,13 +2348,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C46" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46" s="2">
         <v>4</v>
@@ -2365,13 +2365,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>227</v>
+        <v>40</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>228</v>
+        <v>41</v>
       </c>
       <c r="C47" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D47" s="2">
         <v>4</v>
@@ -2382,50 +2382,50 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="C48" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D48" s="2">
         <v>4</v>
       </c>
       <c r="E48" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>126</v>
+        <v>170</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="C49" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49" s="2">
         <v>4</v>
       </c>
       <c r="E49" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>170</v>
+        <v>66</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>171</v>
+        <v>67</v>
       </c>
       <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2">
         <v>3</v>
-      </c>
-      <c r="D50" s="2">
-        <v>4</v>
       </c>
       <c r="E50" s="2">
         <v>0</v>
@@ -2433,10 +2433,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
@@ -2450,10 +2450,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="C52" s="2">
         <v>1</v>
@@ -2467,10 +2467,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="C53" s="2">
         <v>1</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="C54" s="2">
         <v>1</v>
@@ -2501,13 +2501,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>187</v>
+        <v>32</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>188</v>
+        <v>33</v>
       </c>
       <c r="C55" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" s="2">
         <v>3</v>
@@ -2518,13 +2518,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>32</v>
+        <v>242</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>33</v>
+        <v>241</v>
       </c>
       <c r="C56" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D56" s="2">
         <v>3</v>
@@ -2535,13 +2535,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>242</v>
+        <v>93</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>241</v>
+        <v>94</v>
       </c>
       <c r="C57" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D57" s="2">
         <v>3</v>
@@ -2552,10 +2552,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
       <c r="C58" s="2">
         <v>2</v>
@@ -2569,10 +2569,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C59" s="2">
         <v>2</v>
@@ -2586,13 +2586,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="C60" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" s="2">
         <v>3</v>
@@ -2603,10 +2603,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>80</v>
+        <v>212</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>81</v>
+        <v>213</v>
       </c>
       <c r="C61" s="2">
         <v>1</v>
@@ -2620,13 +2620,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
       <c r="C62" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62" s="2">
         <v>3</v>
@@ -2637,10 +2637,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C63" s="2">
         <v>1</v>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>181</v>
+        <v>48</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>182</v>
+        <v>49</v>
       </c>
       <c r="C64" s="2">
         <v>2</v>
@@ -2671,13 +2671,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>64</v>
+        <v>206</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>65</v>
+        <v>207</v>
       </c>
       <c r="C65" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D65" s="2">
         <v>3</v>
@@ -2688,10 +2688,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>48</v>
+        <v>223</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>49</v>
+        <v>224</v>
       </c>
       <c r="C66" s="2">
         <v>2</v>
@@ -2705,13 +2705,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>207</v>
+        <v>83</v>
       </c>
       <c r="C67" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" s="2">
         <v>3</v>
@@ -2722,13 +2722,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>223</v>
+        <v>132</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>224</v>
+        <v>133</v>
       </c>
       <c r="C68" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68" s="2">
         <v>3</v>
@@ -2739,13 +2739,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>82</v>
+        <v>202</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>83</v>
+        <v>203</v>
       </c>
       <c r="C69" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D69" s="2">
         <v>3</v>
@@ -2756,10 +2756,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>132</v>
+        <v>201</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="C70" s="2">
         <v>1</v>
@@ -2773,16 +2773,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>202</v>
+        <v>74</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>203</v>
+        <v>75</v>
       </c>
       <c r="C71" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E71" s="2">
         <v>0</v>
@@ -2790,16 +2790,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>201</v>
+        <v>8</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
       </c>
       <c r="D72" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E72" s="2">
         <v>0</v>
@@ -2807,10 +2807,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C73" s="2">
         <v>1</v>
@@ -2824,13 +2824,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C74" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" s="2">
         <v>2</v>
@@ -2841,10 +2841,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="C75" s="2">
         <v>1</v>
@@ -2858,13 +2858,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C76" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D76" s="2">
         <v>2</v>
@@ -2875,10 +2875,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>159</v>
+        <v>110</v>
       </c>
       <c r="C77" s="2">
         <v>1</v>
@@ -2892,10 +2892,10 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="C78" s="2">
         <v>1</v>
@@ -2909,13 +2909,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="C79" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D79" s="2">
         <v>2</v>
@@ -2926,10 +2926,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="C80" s="2">
         <v>1</v>
@@ -2943,10 +2943,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C81" s="2">
         <v>2</v>
@@ -2960,13 +2960,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C82" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D82" s="2">
         <v>2</v>
@@ -2977,10 +2977,10 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>140</v>
+        <v>215</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>141</v>
+        <v>216</v>
       </c>
       <c r="C83" s="2">
         <v>2</v>
@@ -2994,13 +2994,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="C84" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" s="2">
         <v>2</v>
@@ -3011,10 +3011,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>215</v>
+        <v>30</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>216</v>
+        <v>31</v>
       </c>
       <c r="C85" s="2">
         <v>2</v>
@@ -3028,10 +3028,10 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="C86" s="2">
         <v>1</v>
@@ -3045,13 +3045,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C87" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87" s="2">
         <v>2</v>
@@ -3062,10 +3062,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>152</v>
+        <v>10</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>153</v>
+        <v>11</v>
       </c>
       <c r="C88" s="2">
         <v>1</v>
@@ -3079,10 +3079,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C89" s="2">
         <v>1</v>
@@ -3096,16 +3096,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>10</v>
+        <v>221</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>11</v>
+        <v>222</v>
       </c>
       <c r="C90" s="2">
         <v>1</v>
       </c>
       <c r="D90" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E90" s="2">
         <v>0</v>
@@ -3113,16 +3113,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C91" s="2">
         <v>1</v>
       </c>
       <c r="D91" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E91" s="2">
         <v>0</v>
@@ -3130,10 +3130,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C92" s="2">
         <v>1</v>
@@ -3147,10 +3147,10 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C93" s="2">
         <v>1</v>
@@ -3164,10 +3164,10 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C94" s="2">
         <v>1</v>
@@ -3181,10 +3181,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>58</v>
+        <v>193</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>59</v>
+        <v>194</v>
       </c>
       <c r="C95" s="2">
         <v>1</v>
@@ -3198,10 +3198,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C96" s="2">
         <v>1</v>
@@ -3215,10 +3215,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>219</v>
+        <v>54</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>220</v>
+        <v>55</v>
       </c>
       <c r="C97" s="2">
         <v>1</v>
@@ -3232,10 +3232,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>193</v>
+        <v>90</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>194</v>
+        <v>91</v>
       </c>
       <c r="C98" s="2">
         <v>1</v>
@@ -3249,10 +3249,10 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>44</v>
+        <v>199</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="C99" s="2">
         <v>1</v>
@@ -3266,16 +3266,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>54</v>
+        <v>229</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>55</v>
+        <v>230</v>
       </c>
       <c r="C100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" s="2">
         <v>0</v>
@@ -3283,16 +3283,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="C101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" s="2">
         <v>0</v>
@@ -3300,16 +3300,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2">
         <v>0</v>
@@ -3317,16 +3317,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>199</v>
+        <v>123</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>200</v>
+        <v>124</v>
       </c>
       <c r="C103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" s="2">
         <v>0</v>
@@ -3334,10 +3334,10 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>229</v>
+        <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>230</v>
+        <v>104</v>
       </c>
       <c r="C104" s="2">
         <v>0</v>
@@ -3351,10 +3351,10 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>166</v>
+        <v>60</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>167</v>
+        <v>61</v>
       </c>
       <c r="C105" s="2">
         <v>0</v>
@@ -3368,10 +3368,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
@@ -3385,10 +3385,10 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C107" s="2">
         <v>0</v>
@@ -3402,10 +3402,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="C108" s="2">
         <v>0</v>
@@ -3419,10 +3419,10 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>214</v>
+        <v>24</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C109" s="2">
         <v>0</v>
@@ -3436,10 +3436,10 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="C110" s="2">
         <v>0</v>
@@ -3453,10 +3453,10 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>39</v>
+        <v>157</v>
       </c>
       <c r="C111" s="2">
         <v>0</v>
@@ -3470,10 +3470,10 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="C112" s="2">
         <v>0</v>
@@ -3487,10 +3487,10 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>78</v>
+        <v>177</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="C113" s="2">
         <v>0</v>
@@ -3504,10 +3504,10 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C114" s="2">
         <v>0</v>
@@ -3521,10 +3521,10 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C115" s="2">
         <v>0</v>
@@ -3538,10 +3538,10 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>156</v>
+        <v>28</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>157</v>
+        <v>29</v>
       </c>
       <c r="C116" s="2">
         <v>0</v>
@@ -3550,91 +3550,6 @@
         <v>0</v>
       </c>
       <c r="E116" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C117" s="2">
-        <v>0</v>
-      </c>
-      <c r="D117" s="2">
-        <v>0</v>
-      </c>
-      <c r="E117" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C118" s="2">
-        <v>0</v>
-      </c>
-      <c r="D118" s="2">
-        <v>0</v>
-      </c>
-      <c r="E118" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C119" s="2">
-        <v>0</v>
-      </c>
-      <c r="D119" s="2">
-        <v>0</v>
-      </c>
-      <c r="E119" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C120" s="2">
-        <v>0</v>
-      </c>
-      <c r="D120" s="2">
-        <v>0</v>
-      </c>
-      <c r="E120" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C121" s="2">
-        <v>0</v>
-      </c>
-      <c r="D121" s="2">
-        <v>0</v>
-      </c>
-      <c r="E121" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3650,11 +3565,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>